<commit_message>
code final kernel 32-32 17-20-3 code final seq
</commit_message>
<xml_diff>
--- a/bench.xlsx
+++ b/bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\M1\S2\ProgGraphique\Projet\github\ProjetCUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F01E72-6AD6-4204-B584-5F10CDCD2785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5D3A46-43DA-45D2-B070-F301545CA208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861BEEB7-6285-4C35-8AB7-9362AFA7870C}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,19 +839,19 @@
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="13">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E2" s="13">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F2" s="13">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G2" s="13">
         <v>262</v>
       </c>
       <c r="H2" s="14">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
code final kernel 32-32 17-20-3 \n code final seq \n code final shared 32-32 17-20-3 \n
</commit_message>
<xml_diff>
--- a/bench.xlsx
+++ b/bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\M1\S2\ProgGraphique\Projet\github\ProjetCUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5D3A46-43DA-45D2-B070-F301545CA208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F645AD0C-086A-4352-BCE2-BFD7FE8F7C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861BEEB7-6285-4C35-8AB7-9362AFA7870C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>seq</t>
   </si>
@@ -108,16 +108,46 @@
     <t>5.20</t>
   </si>
   <si>
-    <t>3.14</t>
-  </si>
-  <si>
     <t>3.16</t>
   </si>
   <si>
-    <t>8.33</t>
-  </si>
-  <si>
     <t>8.34</t>
+  </si>
+  <si>
+    <t>4.37</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>8.36</t>
+  </si>
+  <si>
+    <t>2.90</t>
+  </si>
+  <si>
+    <t>1.52</t>
+  </si>
+  <si>
+    <t>3.23</t>
+  </si>
+  <si>
+    <t>2.24</t>
+  </si>
+  <si>
+    <t>5.13</t>
+  </si>
+  <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>3.07</t>
+  </si>
+  <si>
+    <t>5.44</t>
+  </si>
+  <si>
+    <t>4.07</t>
   </si>
 </sst>
 </file>
@@ -792,7 +822,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +916,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>17</v>
@@ -902,16 +932,16 @@
         <v>24</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -950,11 +980,21 @@
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
@@ -962,11 +1002,21 @@
       <c r="C9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="D9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>

</xml_diff>

<commit_message>
code final kernel 32-32 17-20-3 \n code final seq \n code final shared 32-32 17-20-3 \n code final stream 32-32 17-20-3 \n
</commit_message>
<xml_diff>
--- a/bench.xlsx
+++ b/bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\M1\S2\ProgGraphique\Projet\github\ProjetCUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F645AD0C-086A-4352-BCE2-BFD7FE8F7C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA51FF-A7F6-47B5-8891-71DF50AEEEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861BEEB7-6285-4C35-8AB7-9362AFA7870C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>seq</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>4.07</t>
+  </si>
+  <si>
+    <t>4.51</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>5.27</t>
+  </si>
+  <si>
+    <t>3.18</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>8.43</t>
+  </si>
+  <si>
+    <t>8.42</t>
   </si>
 </sst>
 </file>
@@ -822,7 +843,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,8 +1084,12 @@
       <c r="F12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
@@ -1072,11 +1097,21 @@
       <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
+      <c r="D13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>

</xml_diff>

<commit_message>
code final kernel 32-32 17-20-3 \n code final seq \n code final shared 32-32 17-20-3 (pb sur les bordures doubles)\n code final stream 32-32 17-20-3 \n
</commit_message>
<xml_diff>
--- a/bench.xlsx
+++ b/bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\M1\S2\ProgGraphique\Projet\github\ProjetCUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA51FF-A7F6-47B5-8891-71DF50AEEEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA6B62B-CD96-42D2-8ADD-0C2152EA629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861BEEB7-6285-4C35-8AB7-9362AFA7870C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>seq</t>
   </si>
@@ -90,12 +90,6 @@
     <t>time en ms</t>
   </si>
   <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
     <t>0.43</t>
   </si>
   <si>
@@ -126,15 +120,6 @@
     <t>2.90</t>
   </si>
   <si>
-    <t>1.52</t>
-  </si>
-  <si>
-    <t>3.23</t>
-  </si>
-  <si>
-    <t>2.24</t>
-  </si>
-  <si>
     <t>5.13</t>
   </si>
   <si>
@@ -169,6 +154,84 @@
   </si>
   <si>
     <t>8.42</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>2.68</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>3.73</t>
+  </si>
+  <si>
+    <t>2.54</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>1.59</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>2.42</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>1.58</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>2.52</t>
   </si>
 </sst>
 </file>
@@ -502,6 +565,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,18 +587,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -843,7 +906,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +945,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -906,22 +969,32 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="D3" s="11">
+        <v>94</v>
+      </c>
+      <c r="E3" s="11">
+        <v>74</v>
+      </c>
+      <c r="F3" s="11">
+        <v>88</v>
+      </c>
+      <c r="G3" s="11">
+        <v>184</v>
+      </c>
+      <c r="H3" s="12">
+        <v>182</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -937,213 +1010,267 @@
         <v>16</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="D10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
+      <c r="D11" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
+      <c r="D15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
code final kernel 32-32 17-20-3 \n code final seq \n code final shared 32-32 17-20-3 \n code final stream 32-32 17-20-3 \n fin
</commit_message>
<xml_diff>
--- a/bench.xlsx
+++ b/bench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cours\M1\S2\ProgGraphique\Projet\github\ProjetCUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA6B62B-CD96-42D2-8ADD-0C2152EA629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DD6C20-67AB-432B-92FB-29A667F40B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{861BEEB7-6285-4C35-8AB7-9362AFA7870C}"/>
   </bookViews>
@@ -906,7 +906,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>